<commit_message>
small excel bug solve
</commit_message>
<xml_diff>
--- a/A_star_V2/Book1.xlsx
+++ b/A_star_V2/Book1.xlsx
@@ -14,27 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>longest</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
   <si>
     <t>netlist</t>
   </si>
   <si>
+    <t>q25</t>
+  </si>
+  <si>
+    <t>q75</t>
+  </si>
+  <si>
+    <t>shortest</t>
+  </si>
+  <si>
+    <t>total_connected</t>
+  </si>
+  <si>
     <t>true_len</t>
-  </si>
-  <si>
-    <t>longest</t>
-  </si>
-  <si>
-    <t>shortest</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>q25</t>
-  </si>
-  <si>
-    <t>q75</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,83 +423,115 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>24.69230769230769</v>
+      </c>
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="I2">
         <v>963</v>
       </c>
-      <c r="D2">
-        <v>57</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>24.69230769230769</v>
-      </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>37</v>
-      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <v>24.69230769230769</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>37</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="I3">
         <v>963</v>
       </c>
-      <c r="D3">
-        <v>57</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>24.69230769230769</v>
-      </c>
-      <c r="G3">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>24.69230769230769</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="I4">
         <v>963</v>
       </c>
-      <c r="D4">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>57</v>
       </c>
-      <c r="E4">
+      <c r="C5">
+        <v>24.69230769230769</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>37</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>24.69230769230769</v>
-      </c>
-      <c r="G4">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>37</v>
+      <c r="H5">
+        <v>0.78</v>
+      </c>
+      <c r="I5">
+        <v>963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last push for this version, some comments
</commit_message>
<xml_diff>
--- a/A_star_V2/Book1.xlsx
+++ b/A_star_V2/Book1.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s147057\Documents\GitHub\Chips\A_star_V2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FEF090-D46B-4157-9808-9821D79C1A3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>cal_time</t>
   </si>
@@ -135,13 +122,22 @@
   </si>
   <si>
     <t>[((2, 12, 0), (8, 15, 0)), ((13, 15, 0), (15, 1, 0)), ((6, 15, 0), (12, 11, 0)), ((1, 5, 0), (16, 15, 0)), ((11, 5, 0), (7, 12, 0)), ((1, 3, 0), (12, 6, 0)), ((1, 9, 0), (15, 1, 0)), ((13, 7, 0), (13, 15, 0)), ((6, 7, 0), (3, 2, 0)), ((16, 15, 0), (15, 6, 0)), ((7, 8, 0), (9, 8, 0)), ((8, 4, 0), (8, 15, 0)), ((16, 7, 0), (1, 9, 0)), ((15, 1, 0), (4, 14, 0)), ((4, 5, 0), (2, 12, 0)), ((3, 2, 0), (4, 12, 0)), ((15, 6, 0), (11, 15, 0)), ((1, 1, 0), (8, 15, 0)), ((11, 8, 0), (6, 9, 0)), ((15, 1, 0), (10, 1, 0)), ((15, 12, 0), (4, 5, 0)), ((6, 1, 0), (13, 13, 0)), ((6, 9, 0), (15, 3, 0)), ((13, 7, 0), (6, 8, 0)), ((7, 6, 0), (2, 12, 0)), ((15, 8, 0), (6, 14, 0)), ((6, 8, 0), (2, 12, 0)), ((3, 2, 0), (4, 5, 0)), ((1, 9, 0), (12, 2, 0)), ((11, 8, 0), (3, 2, 0)), ((1, 15, 0), (12, 2, 0)), ((4, 14, 0), (6, 3, 0)), ((10, 5, 0), (15, 12, 0)), ((2, 4, 0), (1, 9, 0)), ((12, 3, 0), (11, 8, 0)), ((10, 1, 0), (4, 12, 0)), ((12, 6, 0), (1, 1, 0)), ((6, 14, 0), (9, 8, 0)), ((14, 2, 0), (4, 5, 0)), ((9, 13, 0), (10, 6, 0)), ((4, 5, 0), (8, 4, 0)), ((15, 8, 0), (9, 10, 0)), ((8, 4, 0), (1, 1, 0)), ((2, 6, 0), (15, 12, 0)), ((14, 2, 0), (12, 6, 0)), ((10, 5, 0), (6, 14, 0)), ((6, 1, 0), (8, 4, 0)), ((9, 8, 0), (6, 3, 0)), ((16, 7, 0), (16, 5, 0)), ((15, 8, 0), (3, 2, 0))]</t>
+  </si>
+  <si>
+    <t>[((11, 5, 0), (7, 12, 0)), ((6, 1, 0), (13, 13, 0)), ((11, 8, 0), (3, 2, 0)), ((3, 2, 0), (4, 12, 0)), ((6, 7, 0), (3, 2, 0)), ((16, 7, 0), (16, 5, 0)), ((7, 6, 0), (2, 12, 0)), ((7, 8, 0), (9, 8, 0)), ((10, 1, 0), (4, 12, 0)), ((13, 15, 0), (15, 1, 0)), ((16, 7, 0), (1, 9, 0)), ((15, 8, 0), (9, 10, 0)), ((12, 6, 0), (1, 1, 0)), ((4, 5, 0), (2, 12, 0)), ((15, 6, 0), (11, 15, 0)), ((8, 4, 0), (8, 15, 0)), ((6, 1, 0), (8, 4, 0)), ((16, 15, 0), (15, 6, 0)), ((9, 8, 0), (6, 3, 0)), ((8, 4, 0), (1, 1, 0)), ((1, 3, 0), (12, 6, 0)), ((6, 8, 0), (2, 12, 0)), ((15, 1, 0), (10, 1, 0)), ((11, 8, 0), (6, 9, 0)), ((14, 2, 0), (12, 6, 0)), ((15, 8, 0), (6, 14, 0)), ((6, 14, 0), (9, 8, 0)), ((13, 7, 0), (6, 8, 0)), ((15, 8, 0), (3, 2, 0)), ((10, 5, 0), (15, 12, 0)), ((4, 5, 0), (8, 4, 0)), ((6, 9, 0), (15, 3, 0)), ((9, 13, 0), (10, 6, 0)), ((12, 3, 0), (11, 8, 0)), ((14, 2, 0), (4, 5, 0)), ((10, 5, 0), (6, 14, 0)), ((2, 6, 0), (15, 12, 0)), ((3, 2, 0), (4, 5, 0)), ((4, 14, 0), (6, 3, 0)), ((1, 15, 0), (12, 2, 0)), ((1, 9, 0), (12, 2, 0)), ((1, 5, 0), (16, 15, 0)), ((2, 12, 0), (8, 15, 0)), ((15, 1, 0), (4, 14, 0)), ((13, 7, 0), (13, 15, 0)), ((2, 4, 0), (1, 9, 0)), ((15, 12, 0), (4, 5, 0)), ((1, 1, 0), (8, 15, 0)), ((1, 9, 0), (15, 1, 0)), ((6, 15, 0), (12, 11, 0))]</t>
+  </si>
+  <si>
+    <t>[((2, 12, 0), (8, 15, 0)), ((1, 15, 0), (12, 2, 0)), ((8, 4, 0), (8, 15, 0)), ((16, 7, 0), (16, 5, 0)), ((15, 1, 0), (4, 14, 0)), ((4, 5, 0), (8, 4, 0)), ((15, 8, 0), (6, 14, 0)), ((15, 1, 0), (10, 1, 0)), ((4, 5, 0), (2, 12, 0)), ((1, 9, 0), (15, 1, 0)), ((6, 1, 0), (8, 4, 0)), ((15, 8, 0), (3, 2, 0)), ((16, 15, 0), (15, 6, 0)), ((10, 5, 0), (15, 12, 0)), ((13, 7, 0), (6, 8, 0)), ((1, 1, 0), (8, 15, 0)), ((4, 14, 0), (6, 3, 0)), ((13, 15, 0), (15, 1, 0)), ((3, 2, 0), (4, 12, 0)), ((16, 7, 0), (1, 9, 0)), ((9, 13, 0), (10, 6, 0)), ((15, 8, 0), (9, 10, 0)), ((7, 8, 0), (9, 8, 0)), ((6, 9, 0), (15, 3, 0)), ((1, 9, 0), (12, 2, 0)), ((6, 1, 0), (13, 13, 0)), ((7, 6, 0), (2, 12, 0)), ((10, 1, 0), (4, 12, 0)), ((6, 15, 0), (12, 11, 0)), ((6, 8, 0), (2, 12, 0)), ((11, 8, 0), (6, 9, 0)), ((8, 4, 0), (1, 1, 0)), ((14, 2, 0), (4, 5, 0)), ((12, 3, 0), (11, 8, 0)), ((12, 6, 0), (1, 1, 0)), ((2, 6, 0), (15, 12, 0)), ((14, 2, 0), (12, 6, 0)), ((3, 2, 0), (4, 5, 0)), ((15, 6, 0), (11, 15, 0)), ((6, 14, 0), (9, 8, 0)), ((2, 4, 0), (1, 9, 0)), ((1, 5, 0), (16, 15, 0)), ((10, 5, 0), (6, 14, 0)), ((6, 7, 0), (3, 2, 0)), ((11, 8, 0), (3, 2, 0)), ((1, 3, 0), (12, 6, 0)), ((15, 12, 0), (4, 5, 0)), ((9, 8, 0), (6, 3, 0)), ((13, 7, 0), (13, 15, 0)), ((11, 5, 0), (7, 12, 0))]</t>
+  </si>
+  <si>
+    <t>[((3, 2, 0), (4, 12, 0)), ((1, 9, 0), (12, 2, 0)), ((1, 5, 0), (16, 15, 0)), ((13, 7, 0), (6, 8, 0)), ((2, 12, 0), (8, 15, 0)), ((16, 7, 0), (16, 5, 0)), ((12, 3, 0), (11, 8, 0)), ((7, 8, 0), (9, 8, 0)), ((8, 4, 0), (8, 15, 0)), ((3, 2, 0), (4, 5, 0)), ((15, 8, 0), (3, 2, 0)), ((15, 1, 0), (10, 1, 0)), ((1, 15, 0), (12, 2, 0)), ((6, 8, 0), (2, 12, 0)), ((9, 13, 0), (10, 6, 0)), ((2, 4, 0), (1, 9, 0)), ((7, 6, 0), (2, 12, 0)), ((14, 2, 0), (12, 6, 0)), ((6, 7, 0), (3, 2, 0)), ((9, 8, 0), (6, 3, 0)), ((4, 14, 0), (6, 3, 0)), ((1, 3, 0), (12, 6, 0)), ((16, 7, 0), (1, 9, 0)), ((2, 6, 0), (15, 12, 0)), ((15, 12, 0), (4, 5, 0)), ((16, 15, 0), (15, 6, 0)), ((13, 15, 0), (15, 1, 0)), ((11, 5, 0), (7, 12, 0)), ((6, 9, 0), (15, 3, 0)), ((11, 8, 0), (6, 9, 0)), ((1, 1, 0), (8, 15, 0)), ((15, 1, 0), (4, 14, 0)), ((1, 9, 0), (15, 1, 0)), ((15, 6, 0), (11, 15, 0)), ((10, 5, 0), (6, 14, 0)), ((4, 5, 0), (2, 12, 0)), ((6, 14, 0), (9, 8, 0)), ((11, 8, 0), (3, 2, 0)), ((6, 1, 0), (8, 4, 0)), ((8, 4, 0), (1, 1, 0)), ((13, 7, 0), (13, 15, 0)), ((15, 8, 0), (9, 10, 0)), ((10, 5, 0), (15, 12, 0)), ((15, 8, 0), (6, 14, 0)), ((14, 2, 0), (4, 5, 0)), ((6, 1, 0), (13, 13, 0)), ((4, 5, 0), (8, 4, 0)), ((10, 1, 0), (4, 12, 0)), ((6, 15, 0), (12, 11, 0)), ((12, 6, 0), (1, 1, 0))]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,14 +200,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -258,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,27 +278,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,24 +312,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -535,16 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23:M45"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,12 +529,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>35.723562955856323</v>
+        <v>35.72356295585632</v>
       </c>
       <c r="C2">
         <v>2.4</v>
@@ -614,12 +564,12 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>37.237612009048462</v>
+        <v>37.23761200904846</v>
       </c>
       <c r="C3">
         <v>2.4</v>
@@ -649,21 +599,21 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>97.803836584091187</v>
+        <v>97.80383658409119</v>
       </c>
       <c r="C4">
-        <v>2.8003629764065341</v>
+        <v>2.800362976406534</v>
       </c>
       <c r="D4">
         <v>63</v>
       </c>
       <c r="E4">
-        <v>26.603448275862071</v>
+        <v>26.60344827586207</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -678,27 +628,27 @@
         <v>2</v>
       </c>
       <c r="K4">
-        <v>0.96666666666666667</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="L4">
         <v>1543</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>261.01125884056091</v>
+        <v>261.0112588405609</v>
       </c>
       <c r="C5">
-        <v>2.7687165775401068</v>
+        <v>2.768716577540107</v>
       </c>
       <c r="D5">
         <v>74</v>
       </c>
       <c r="E5">
-        <v>30.014492753623191</v>
+        <v>30.01449275362319</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -713,27 +663,27 @@
         <v>3</v>
       </c>
       <c r="K5">
-        <v>0.98571428571428577</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="L5">
         <v>2071</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>156.82492876052859</v>
+        <v>156.8249287605286</v>
       </c>
       <c r="C6">
-        <v>2.6790830945558741</v>
+        <v>2.679083094555874</v>
       </c>
       <c r="D6">
         <v>69</v>
       </c>
       <c r="E6">
-        <v>28.333333333333329</v>
+        <v>28.33333333333333</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -748,18 +698,18 @@
         <v>3</v>
       </c>
       <c r="K6">
-        <v>0.94285714285714284</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="L6">
         <v>1870</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>27.462228536605831</v>
+        <v>27.46222853660583</v>
       </c>
       <c r="C7">
         <v>2.535714285714286</v>
@@ -768,7 +718,7 @@
         <v>69</v>
       </c>
       <c r="E7">
-        <v>22.659574468085111</v>
+        <v>22.65957446808511</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -783,18 +733,18 @@
         <v>3</v>
       </c>
       <c r="K7">
-        <v>0.67142857142857137</v>
+        <v>0.6714285714285714</v>
       </c>
       <c r="L7">
         <v>1065</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>27.330292940139771</v>
+        <v>27.33029294013977</v>
       </c>
       <c r="C8">
         <v>2.535714285714286</v>
@@ -803,7 +753,7 @@
         <v>69</v>
       </c>
       <c r="E8">
-        <v>22.659574468085111</v>
+        <v>22.65957446808511</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -818,27 +768,27 @@
         <v>3</v>
       </c>
       <c r="K8">
-        <v>0.67142857142857137</v>
+        <v>0.6714285714285714</v>
       </c>
       <c r="L8">
         <v>1065</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>148.06099271774289</v>
+        <v>148.0609927177429</v>
       </c>
       <c r="C9">
-        <v>2.6093333333333328</v>
+        <v>2.609333333333333</v>
       </c>
       <c r="D9">
         <v>64</v>
       </c>
       <c r="E9">
-        <v>28.362318840579711</v>
+        <v>28.36231884057971</v>
       </c>
       <c r="F9">
         <v>6</v>
@@ -853,21 +803,21 @@
         <v>3</v>
       </c>
       <c r="K9">
-        <v>0.98571428571428577</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="L9">
         <v>1957</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>167.99852871894839</v>
+        <v>167.9985287189484</v>
       </c>
       <c r="C10">
-        <v>2.7330508474576272</v>
+        <v>2.733050847457627</v>
       </c>
       <c r="D10">
         <v>82</v>
@@ -894,7 +844,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -908,7 +858,7 @@
         <v>54</v>
       </c>
       <c r="E11">
-        <v>26.661764705882351</v>
+        <v>26.66176470588235</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -923,27 +873,27 @@
         <v>3</v>
       </c>
       <c r="K11">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L11">
         <v>1813</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>97.602967977523804</v>
+        <v>97.6029679775238</v>
       </c>
       <c r="C12">
-        <v>2.6580732700135679</v>
+        <v>2.658073270013568</v>
       </c>
       <c r="D12">
         <v>87</v>
       </c>
       <c r="E12">
-        <v>28.808823529411761</v>
+        <v>28.80882352941176</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -958,13 +908,13 @@
         <v>3</v>
       </c>
       <c r="K12">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L12">
         <v>1959</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -972,7 +922,7 @@
         <v>216.0549445152283</v>
       </c>
       <c r="C13">
-        <v>2.7318116975748929</v>
+        <v>2.731811697574893</v>
       </c>
       <c r="D13">
         <v>74</v>
@@ -993,13 +943,13 @@
         <v>3</v>
       </c>
       <c r="K13">
-        <v>0.91428571428571426</v>
+        <v>0.9142857142857143</v>
       </c>
       <c r="L13">
         <v>1915</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1007,13 +957,13 @@
         <v>109.8809022903442</v>
       </c>
       <c r="C14">
-        <v>2.8175765645805591</v>
+        <v>2.817576564580559</v>
       </c>
       <c r="D14">
         <v>81</v>
       </c>
       <c r="E14">
-        <v>30.666666666666671</v>
+        <v>30.66666666666667</v>
       </c>
       <c r="F14">
         <v>6</v>
@@ -1028,18 +978,18 @@
         <v>3</v>
       </c>
       <c r="K14">
-        <v>0.98571428571428577</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="L14">
         <v>2116</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>99.462884664535522</v>
+        <v>99.46288466453552</v>
       </c>
       <c r="C15">
         <v>2.663989290495314</v>
@@ -1048,7 +998,7 @@
         <v>70</v>
       </c>
       <c r="E15">
-        <v>28.840579710144929</v>
+        <v>28.84057971014493</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -1063,13 +1013,13 @@
         <v>3</v>
       </c>
       <c r="K15">
-        <v>0.98571428571428577</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="L15">
         <v>1990</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1077,13 +1027,13 @@
         <v>146.1210849285126</v>
       </c>
       <c r="C16">
-        <v>2.6616643929058661</v>
+        <v>2.661664392905866</v>
       </c>
       <c r="D16">
         <v>74</v>
       </c>
       <c r="E16">
-        <v>28.691176470588239</v>
+        <v>28.69117647058824</v>
       </c>
       <c r="F16">
         <v>6</v>
@@ -1098,27 +1048,27 @@
         <v>3</v>
       </c>
       <c r="K16">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L16">
         <v>1951</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>147.46631932258609</v>
+        <v>147.4663193225861</v>
       </c>
       <c r="C17">
-        <v>2.4691195795006569</v>
+        <v>2.469119579500657</v>
       </c>
       <c r="D17">
         <v>58</v>
       </c>
       <c r="E17">
-        <v>26.842857142857142</v>
+        <v>26.84285714285714</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1139,21 +1089,21 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>169.47767996788019</v>
+        <v>169.4776799678802</v>
       </c>
       <c r="C18">
-        <v>2.9690140845070419</v>
+        <v>2.969014084507042</v>
       </c>
       <c r="D18">
         <v>84</v>
       </c>
       <c r="E18">
-        <v>31.939393939393941</v>
+        <v>31.93939393939394</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -1168,21 +1118,21 @@
         <v>3</v>
       </c>
       <c r="K18">
-        <v>0.94285714285714284</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="L18">
         <v>2108</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>82.526550054550171</v>
+        <v>82.52655005455017</v>
       </c>
       <c r="C19">
-        <v>2.4873096446700509</v>
+        <v>2.487309644670051</v>
       </c>
       <c r="D19">
         <v>59</v>
@@ -1212,7 +1162,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1220,7 +1170,7 @@
         <v>214.7776594161987</v>
       </c>
       <c r="C20">
-        <v>2.8011049723756911</v>
+        <v>2.801104972375691</v>
       </c>
       <c r="D20">
         <v>69</v>
@@ -1244,27 +1194,27 @@
         <v>12</v>
       </c>
       <c r="K20">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L20">
         <v>2028</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>301.80901551246637</v>
+        <v>301.8090155124664</v>
       </c>
       <c r="C21">
-        <v>2.7086183310533509</v>
+        <v>2.708618331053351</v>
       </c>
       <c r="D21">
         <v>76</v>
       </c>
       <c r="E21">
-        <v>29.552238805970148</v>
+        <v>29.55223880597015</v>
       </c>
       <c r="F21">
         <v>6</v>
@@ -1282,18 +1232,18 @@
         <v>13</v>
       </c>
       <c r="K21">
-        <v>0.95714285714285718</v>
+        <v>0.9571428571428572</v>
       </c>
       <c r="L21">
         <v>1980</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>324.15747427940369</v>
+        <v>324.1574742794037</v>
       </c>
       <c r="C22">
         <v>2.822625698324023</v>
@@ -1302,7 +1252,7 @@
         <v>82</v>
       </c>
       <c r="E22">
-        <v>30.164179104477611</v>
+        <v>30.16417910447761</v>
       </c>
       <c r="F22">
         <v>6</v>
@@ -1320,18 +1270,18 @@
         <v>14</v>
       </c>
       <c r="K22">
-        <v>0.95714285714285718</v>
+        <v>0.9571428571428572</v>
       </c>
       <c r="L22">
         <v>2021</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>355.62372088432312</v>
+        <v>355.6237208843231</v>
       </c>
       <c r="C23">
         <v>2.526748971193415</v>
@@ -1340,7 +1290,7 @@
         <v>65</v>
       </c>
       <c r="E23">
-        <v>27.492537313432841</v>
+        <v>27.49253731343284</v>
       </c>
       <c r="F23">
         <v>6</v>
@@ -1358,18 +1308,18 @@
         <v>15</v>
       </c>
       <c r="K23">
-        <v>0.95714285714285718</v>
+        <v>0.9571428571428572</v>
       </c>
       <c r="L23">
         <v>1842</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>142.52325224876401</v>
+        <v>142.523252248764</v>
       </c>
       <c r="C24">
         <v>2.60079575596817</v>
@@ -1378,7 +1328,7 @@
         <v>67</v>
       </c>
       <c r="E24">
-        <v>28.420289855072461</v>
+        <v>28.42028985507246</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -1396,18 +1346,18 @@
         <v>16</v>
       </c>
       <c r="K24">
-        <v>0.98571428571428577</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="L24">
         <v>1961</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>175.81148481369021</v>
+        <v>175.8114848136902</v>
       </c>
       <c r="C25">
         <v>2.978975032851511</v>
@@ -1416,7 +1366,7 @@
         <v>91</v>
       </c>
       <c r="E25">
-        <v>32.385714285714293</v>
+        <v>32.38571428571429</v>
       </c>
       <c r="F25">
         <v>6</v>
@@ -1440,12 +1390,12 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>206.28621959686279</v>
+        <v>206.2862195968628</v>
       </c>
       <c r="C26">
         <v>2.5</v>
@@ -1472,18 +1422,18 @@
         <v>18</v>
       </c>
       <c r="K26">
-        <v>0.91428571428571426</v>
+        <v>0.9142857142857143</v>
       </c>
       <c r="L26">
         <v>1700</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>203.01802182197571</v>
+        <v>203.0180218219757</v>
       </c>
       <c r="C27">
         <v>2.666666666666667</v>
@@ -1492,7 +1442,7 @@
         <v>77</v>
       </c>
       <c r="E27">
-        <v>29.333333333333329</v>
+        <v>29.33333333333333</v>
       </c>
       <c r="F27">
         <v>6</v>
@@ -1510,21 +1460,21 @@
         <v>19</v>
       </c>
       <c r="K27">
-        <v>0.94285714285714284</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="L27">
         <v>1936</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>281.74986386299128</v>
+        <v>281.7498638629913</v>
       </c>
       <c r="C28">
-        <v>2.8746355685131202</v>
+        <v>2.87463556851312</v>
       </c>
       <c r="D28">
         <v>60</v>
@@ -1548,21 +1498,21 @@
         <v>20</v>
       </c>
       <c r="K28">
-        <v>0.91428571428571426</v>
+        <v>0.9142857142857143</v>
       </c>
       <c r="L28">
         <v>1972</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>132.87544536590579</v>
+        <v>132.8754453659058</v>
       </c>
       <c r="C29">
-        <v>2.8421052631578951</v>
+        <v>2.842105263157895</v>
       </c>
       <c r="D29">
         <v>75</v>
@@ -1586,21 +1536,21 @@
         <v>21</v>
       </c>
       <c r="K29">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L29">
         <v>2052</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>187.47512054443359</v>
+        <v>187.4751205444336</v>
       </c>
       <c r="C30">
-        <v>2.8050847457627119</v>
+        <v>2.805084745762712</v>
       </c>
       <c r="D30">
         <v>63</v>
@@ -1624,27 +1574,27 @@
         <v>22</v>
       </c>
       <c r="K30">
-        <v>0.94285714285714284</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="L30">
         <v>1986</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>151.83277630805969</v>
+        <v>151.8327763080597</v>
       </c>
       <c r="C31">
-        <v>2.7811217510259918</v>
+        <v>2.781121751025992</v>
       </c>
       <c r="D31">
         <v>80</v>
       </c>
       <c r="E31">
-        <v>29.897058823529409</v>
+        <v>29.89705882352941</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -1662,13 +1612,13 @@
         <v>23</v>
       </c>
       <c r="K31">
-        <v>0.97142857142857142</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="L31">
         <v>2033</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1700,27 +1650,27 @@
         <v>24</v>
       </c>
       <c r="K32">
-        <v>0.96666666666666667</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="L32">
         <v>1615</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>152.04369425773621</v>
+        <v>152.0436942577362</v>
       </c>
       <c r="C33">
-        <v>2.7131931166347991</v>
+        <v>2.713193116634799</v>
       </c>
       <c r="D33">
         <v>69</v>
       </c>
       <c r="E33">
-        <v>25.339285714285719</v>
+        <v>25.33928571428572</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -1738,18 +1688,18 @@
         <v>25</v>
       </c>
       <c r="K33">
-        <v>0.93333333333333335</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="L33">
         <v>1419</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>85.519909381866455</v>
+        <v>85.51990938186646</v>
       </c>
       <c r="C34">
         <v>2.692041522491349</v>
@@ -1782,21 +1732,21 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>66.605208396911621</v>
+        <v>66.60520839691162</v>
       </c>
       <c r="C35">
-        <v>2.9204152249134951</v>
+        <v>2.920415224913495</v>
       </c>
       <c r="D35">
         <v>71</v>
       </c>
       <c r="E35">
-        <v>28.133333333333329</v>
+        <v>28.13333333333333</v>
       </c>
       <c r="F35">
         <v>5</v>
@@ -1820,15 +1770,15 @@
         <v>1688</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>80.164963960647583</v>
+        <v>80.16496396064758</v>
       </c>
       <c r="C36">
-        <v>2.9390681003584231</v>
+        <v>2.939068100358423</v>
       </c>
       <c r="D36">
         <v>74</v>
@@ -1852,27 +1802,27 @@
         <v>28</v>
       </c>
       <c r="K36">
-        <v>0.96666666666666667</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="L36">
         <v>1640</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>76.489118099212646</v>
+        <v>76.48911809921265</v>
       </c>
       <c r="C37">
-        <v>2.8581314878892732</v>
+        <v>2.858131487889273</v>
       </c>
       <c r="D37">
         <v>61</v>
       </c>
       <c r="E37">
-        <v>27.533333333333331</v>
+        <v>27.53333333333333</v>
       </c>
       <c r="F37">
         <v>5</v>
@@ -1896,7 +1846,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1904,7 +1854,7 @@
         <v>53.63319730758667</v>
       </c>
       <c r="C38">
-        <v>2.4700000000000002</v>
+        <v>2.47</v>
       </c>
       <c r="D38">
         <v>68</v>
@@ -1934,7 +1884,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1942,7 +1892,7 @@
         <v>170.6309189796448</v>
       </c>
       <c r="C39">
-        <v>2.8074866310160429</v>
+        <v>2.807486631016043</v>
       </c>
       <c r="D39">
         <v>72</v>
@@ -1972,12 +1922,12 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>68.445927143096924</v>
+        <v>68.44592714309692</v>
       </c>
       <c r="C40">
         <v>2.71</v>
@@ -1986,7 +1936,7 @@
         <v>66</v>
       </c>
       <c r="E40">
-        <v>32.520000000000003</v>
+        <v>32.52</v>
       </c>
       <c r="F40">
         <v>4</v>
@@ -2010,12 +1960,12 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>55.168322324752808</v>
+        <v>55.16832232475281</v>
       </c>
       <c r="C41">
         <v>2.626666666666666</v>
@@ -2048,7 +1998,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2056,7 +2006,7 @@
         <v>41.94691276550293</v>
       </c>
       <c r="C42">
-        <v>2.4833333333333329</v>
+        <v>2.483333333333333</v>
       </c>
       <c r="D42">
         <v>63</v>
@@ -2086,7 +2036,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2094,13 +2044,13 @@
         <v>154.488322019577</v>
       </c>
       <c r="C43">
-        <v>2.6576086956521738</v>
+        <v>2.657608695652174</v>
       </c>
       <c r="D43">
         <v>69</v>
       </c>
       <c r="E43">
-        <v>31.212765957446809</v>
+        <v>31.21276595744681</v>
       </c>
       <c r="F43">
         <v>4</v>
@@ -2118,10 +2068,124 @@
         <v>35</v>
       </c>
       <c r="K43">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="L43">
         <v>1467</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>42.10082268714905</v>
+      </c>
+      <c r="C44">
+        <v>2.863333333333333</v>
+      </c>
+      <c r="D44">
+        <v>77</v>
+      </c>
+      <c r="E44">
+        <v>34.36</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>29</v>
+      </c>
+      <c r="H44">
+        <v>37</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44" t="s">
+        <v>36</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>85.43693900108337</v>
+      </c>
+      <c r="C45">
+        <v>2.536666666666667</v>
+      </c>
+      <c r="D45">
+        <v>71</v>
+      </c>
+      <c r="E45">
+        <v>30.44</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>17</v>
+      </c>
+      <c r="H45">
+        <v>48</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>50.91376399993896</v>
+      </c>
+      <c r="C46">
+        <v>2.576666666666667</v>
+      </c>
+      <c r="D46">
+        <v>74</v>
+      </c>
+      <c r="E46">
+        <v>30.92</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>33</v>
+      </c>
+      <c r="H46">
+        <v>41</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>